<commit_message>
Cambios tileset y arreglo carga de tiles peques: engarzado normal
</commit_message>
<xml_diff>
--- a/ProyectoII/bmps/TILES Y CARACTERES.xlsx
+++ b/ProyectoII/bmps/TILES Y CARACTERES.xlsx
@@ -231,27 +231,12 @@
     <t>Ø</t>
   </si>
   <si>
-    <t>ő</t>
-  </si>
-  <si>
-    <t>ȫ</t>
-  </si>
-  <si>
-    <t>δ</t>
-  </si>
-  <si>
-    <t>σ</t>
-  </si>
-  <si>
     <t>BOSQUE E</t>
   </si>
   <si>
     <t>LAGO O</t>
   </si>
   <si>
-    <t>ē</t>
-  </si>
-  <si>
     <t>ë</t>
   </si>
   <si>
@@ -288,21 +273,9 @@
     <t>i</t>
   </si>
   <si>
-    <t>ľ</t>
-  </si>
-  <si>
-    <t>Ĭ</t>
-  </si>
-  <si>
     <t>Ũ</t>
   </si>
   <si>
-    <t>ų</t>
-  </si>
-  <si>
-    <t>ă</t>
-  </si>
-  <si>
     <t>å</t>
   </si>
   <si>
@@ -394,6 +367,33 @@
   </si>
   <si>
     <t>Ð</t>
+  </si>
+  <si>
+    <t>×</t>
+  </si>
+  <si>
+    <t>©</t>
+  </si>
+  <si>
+    <t>¬</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>¿</t>
+  </si>
+  <si>
+    <t>¼</t>
+  </si>
+  <si>
+    <t>½</t>
+  </si>
+  <si>
+    <t>¾</t>
+  </si>
+  <si>
+    <t>Á</t>
   </si>
 </sst>
 </file>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C1">
         <v>21</v>
@@ -943,7 +943,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="C2">
         <v>57</v>
@@ -955,7 +955,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C3">
         <v>58</v>
@@ -967,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C4" s="18">
         <v>20</v>
@@ -979,7 +979,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="C5">
         <v>22</v>
@@ -992,7 +992,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>25</v>
@@ -1004,7 +1004,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C7">
         <v>23</v>
@@ -1016,7 +1016,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C8">
         <v>24</v>
@@ -1028,7 +1028,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C9">
         <v>26</v>
@@ -1042,7 +1042,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>29</v>
@@ -1054,7 +1054,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C11">
         <v>27</v>
@@ -1067,22 +1067,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C12">
         <v>28</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C13">
         <v>31</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C14">
         <v>33</v>
@@ -1106,7 +1106,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C15">
         <v>30</v>
@@ -1118,7 +1118,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C16">
         <v>32</v>
@@ -1130,7 +1130,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C17">
         <v>38</v>
@@ -1142,7 +1142,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C18">
         <v>36</v>
@@ -1154,7 +1154,7 @@
         <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C19">
         <v>35</v>
@@ -1166,7 +1166,7 @@
         <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C20">
         <v>37</v>
@@ -1178,7 +1178,7 @@
         <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C21">
         <v>34</v>
@@ -1265,7 +1265,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -1277,14 +1277,14 @@
         <v>21</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C29">
         <v>11</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1292,7 +1292,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -1361,7 +1361,7 @@
         <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1373,7 +1373,7 @@
         <v>46</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -1385,7 +1385,7 @@
         <v>47</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -1397,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1409,7 +1409,7 @@
         <v>28</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C41">
         <v>41</v>
@@ -1421,7 +1421,7 @@
         <v>29</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C42">
         <v>43</v>
@@ -1433,7 +1433,7 @@
         <v>30</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C43">
         <v>40</v>
@@ -1445,7 +1445,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C44">
         <v>42</v>
@@ -1457,7 +1457,7 @@
         <v>31</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C45">
         <v>48</v>
@@ -1469,7 +1469,7 @@
         <v>32</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C46">
         <v>49</v>
@@ -1481,7 +1481,7 @@
         <v>33</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C47">
         <v>50</v>
@@ -1493,7 +1493,7 @@
         <v>34</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C48">
         <v>51</v>
@@ -1505,7 +1505,7 @@
         <v>35</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="C49">
         <v>54</v>
@@ -1517,7 +1517,7 @@
         <v>36</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C50">
         <v>52</v>
@@ -1529,7 +1529,7 @@
         <v>37</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C51">
         <v>55</v>
@@ -1541,7 +1541,7 @@
         <v>38</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="C52">
         <v>53</v>
@@ -1554,7 +1554,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C53">
         <v>56</v>
@@ -1566,7 +1566,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C54">
         <v>45</v>
@@ -1578,7 +1578,7 @@
         <v>41</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C55">
         <v>44</v>
@@ -1587,10 +1587,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C56">
         <v>46</v>
@@ -1602,7 +1602,7 @@
         <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C57">
         <v>47</v>
@@ -1614,7 +1614,7 @@
         <v>52</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C58">
         <v>17</v>
@@ -1626,7 +1626,7 @@
         <v>53</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C59">
         <v>16</v>
@@ -1638,7 +1638,7 @@
         <v>54</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C60">
         <v>18</v>
@@ -1650,7 +1650,7 @@
         <v>55</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="C61">
         <v>19</v>
@@ -1662,7 +1662,7 @@
         <v>56</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D62" s="21"/>
     </row>

</xml_diff>